<commit_message>
Bring up for board 2 complete
</commit_message>
<xml_diff>
--- a/2 Architecture/DDS Tone Shield Major Component BOM  REV 03.xlsx
+++ b/2 Architecture/DDS Tone Shield Major Component BOM  REV 03.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Major Components " sheetId="1" r:id="rId1"/>
     <sheet name="Component Comparision" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -692,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C16:C17"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1035,6 +1035,68 @@
       <c r="H15">
         <f>SUM(H8:H12)</f>
         <v>14.45</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <f>1.27*E21</f>
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" ref="F22:F26" si="0">1.27*E22</f>
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="13">
+        <v>4</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="0"/>
+        <v>5.08</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="13">
+        <v>5</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="0"/>
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="13">
+        <v>6</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="0"/>
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="13">
+        <v>7</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="0"/>
+        <v>8.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test Writeup, Code for attiny
Added base firmware for attiny85 under architecture.
Added a single point test writeup for signal seen.
Added screenshots of signals to show what was generated.
Commented code
</commit_message>
<xml_diff>
--- a/2 Architecture/DDS Tone Shield Major Component BOM  REV 03.xlsx
+++ b/2 Architecture/DDS Tone Shield Major Component BOM  REV 03.xlsx
@@ -695,7 +695,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="G27" sqref="G26:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1037,67 +1037,24 @@
         <v>14.45</v>
       </c>
     </row>
-    <row r="20" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <f>1.27*E21</f>
-        <v>2.54</v>
-      </c>
-    </row>
     <row r="22" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22" s="13">
-        <f t="shared" ref="F22:F26" si="0">1.27*E22</f>
-        <v>3.81</v>
-      </c>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E23" s="13">
-        <v>4</v>
-      </c>
-      <c r="F23" s="13">
-        <f t="shared" si="0"/>
-        <v>5.08</v>
-      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E24" s="13">
-        <v>5</v>
-      </c>
-      <c r="F24" s="13">
-        <f t="shared" si="0"/>
-        <v>6.35</v>
-      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E25" s="13">
-        <v>6</v>
-      </c>
-      <c r="F25" s="13">
-        <f t="shared" si="0"/>
-        <v>7.62</v>
-      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="5:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E26" s="13">
-        <v>7</v>
-      </c>
-      <c r="F26" s="13">
-        <f t="shared" si="0"/>
-        <v>8.89</v>
-      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>